<commit_message>
Result tables updated after AutLvls changed
</commit_message>
<xml_diff>
--- a/data/results/00_descriptiveResults_singleTC.xlsx
+++ b/data/results/00_descriptiveResults_singleTC.xlsx
@@ -20,7 +20,424 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="278">
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC02_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC03_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC04_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC05_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC06_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC07_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC08_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC09_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC10_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC11_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC12_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC06_AvailReasonCorrect_rel</t>
+  </si>
+  <si>
+    <t>TC10_AvailReasonCorrect_rel</t>
+  </si>
+  <si>
+    <t>TC12_AvailReasonCorrect_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC02_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC03_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC04_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC05_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC06_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC07_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC08_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC09_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC10_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC11_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC12_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC02_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC03_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC04_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC05_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC06_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC07_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC08_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC09_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC10_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC11_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC12_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC02_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC03_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC04_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC05_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC06_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC07_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC08_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC09_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC10_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC11_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC12_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC02_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC03_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC04_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC05_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC06_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC07_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC08_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC09_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC10_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC11_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC12_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC03_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC05_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC09_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC10_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC11_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC12_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
   <si>
     <t>Exp</t>
   </si>
@@ -457,7 +874,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -472,11 +889,18 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -485,6 +909,13 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,52 +948,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>139</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>140</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>8</v>
+        <v>147</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>9</v>
+        <v>148</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>10</v>
+        <v>149</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>11</v>
+        <v>150</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>12</v>
+        <v>151</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>13</v>
+        <v>152</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>14</v>
+        <v>153</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>15</v>
+        <v>154</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>16</v>
+        <v>155</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>17</v>
+        <v>156</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>18</v>
+        <v>157</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>19</v>
+        <v>158</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>20</v>
+        <v>159</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>21</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2">
@@ -570,7 +1001,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>2</v>
+        <v>141</v>
       </c>
       <c r="C2" s="0">
         <v>84.939999999999998</v>
@@ -620,7 +1051,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>3</v>
+        <v>142</v>
       </c>
       <c r="C3" s="0">
         <v>84.939999999999998</v>
@@ -670,7 +1101,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>4</v>
+        <v>143</v>
       </c>
       <c r="C4" s="0">
         <v>81.819999999999993</v>
@@ -720,7 +1151,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>5</v>
+        <v>144</v>
       </c>
       <c r="C5" s="0">
         <v>74.700000000000003</v>
@@ -770,7 +1201,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>6</v>
+        <v>145</v>
       </c>
       <c r="C6" s="0">
         <v>85.319999999999993</v>
@@ -820,7 +1251,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>7</v>
+        <v>146</v>
       </c>
       <c r="C7" s="0">
         <v>71.430000000000007</v>
@@ -885,25 +1316,25 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>22</v>
+        <v>161</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>23</v>
+        <v>162</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>30</v>
+        <v>169</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>31</v>
+        <v>170</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>32</v>
+        <v>171</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>33</v>
+        <v>172</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>34</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2">
@@ -911,7 +1342,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>24</v>
+        <v>163</v>
       </c>
       <c r="C2" s="0">
         <v>62.82</v>
@@ -934,7 +1365,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>25</v>
+        <v>164</v>
       </c>
       <c r="C3" s="0">
         <v>75.640000000000001</v>
@@ -957,7 +1388,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>26</v>
+        <v>165</v>
       </c>
       <c r="C4" s="0">
         <v>62.630000000000003</v>
@@ -980,7 +1411,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>27</v>
+        <v>166</v>
       </c>
       <c r="C5" s="0">
         <v>55.950000000000003</v>
@@ -1003,7 +1434,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>28</v>
+        <v>167</v>
       </c>
       <c r="C6" s="0">
         <v>41.270000000000003</v>
@@ -1026,7 +1457,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>29</v>
+        <v>168</v>
       </c>
       <c r="C7" s="0">
         <v>23.809999999999999</v>
@@ -1073,52 +1504,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>35</v>
+        <v>174</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>36</v>
+        <v>175</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>43</v>
+        <v>182</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>44</v>
+        <v>183</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>45</v>
+        <v>184</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>46</v>
+        <v>185</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>47</v>
+        <v>186</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>48</v>
+        <v>187</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>49</v>
+        <v>188</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>50</v>
+        <v>189</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>51</v>
+        <v>190</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>52</v>
+        <v>191</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>53</v>
+        <v>192</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>54</v>
+        <v>193</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>55</v>
+        <v>194</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>56</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2">
@@ -1126,7 +1557,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>37</v>
+        <v>176</v>
       </c>
       <c r="C2" s="0">
         <v>98.719999999999999</v>
@@ -1176,7 +1607,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>38</v>
+        <v>177</v>
       </c>
       <c r="C3" s="0">
         <v>97.120000000000005</v>
@@ -1226,7 +1657,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>39</v>
+        <v>178</v>
       </c>
       <c r="C4" s="0">
         <v>95.200000000000003</v>
@@ -1276,7 +1707,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>40</v>
+        <v>179</v>
       </c>
       <c r="C5" s="0">
         <v>87.5</v>
@@ -1326,10 +1757,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>41</v>
+        <v>180</v>
       </c>
       <c r="C6" s="0">
-        <v>95.239999999999995</v>
+        <v>95.629999999999995</v>
       </c>
       <c r="D6" s="0">
         <v>100</v>
@@ -1365,7 +1796,7 @@
         <v>100</v>
       </c>
       <c r="O6" s="0">
-        <v>90.480000000000004</v>
+        <v>95.239999999999995</v>
       </c>
       <c r="P6" s="0">
         <v>21</v>
@@ -1376,7 +1807,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>42</v>
+        <v>181</v>
       </c>
       <c r="C7" s="0">
         <v>84.920000000000002</v>
@@ -1450,52 +1881,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>57</v>
+        <v>196</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>58</v>
+        <v>197</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>65</v>
+        <v>204</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>66</v>
+        <v>205</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>67</v>
+        <v>206</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>68</v>
+        <v>207</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>69</v>
+        <v>208</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>70</v>
+        <v>209</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>71</v>
+        <v>210</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>72</v>
+        <v>211</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>73</v>
+        <v>212</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>74</v>
+        <v>213</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>75</v>
+        <v>214</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>76</v>
+        <v>215</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>77</v>
+        <v>216</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>78</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2">
@@ -1503,7 +1934,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>59</v>
+        <v>198</v>
       </c>
       <c r="C2" s="0">
         <v>98.719999999999999</v>
@@ -1553,7 +1984,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>60</v>
+        <v>199</v>
       </c>
       <c r="C3" s="0">
         <v>96.790000000000006</v>
@@ -1603,7 +2034,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>61</v>
+        <v>200</v>
       </c>
       <c r="C4" s="0">
         <v>90.400000000000006</v>
@@ -1653,7 +2084,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>62</v>
+        <v>201</v>
       </c>
       <c r="C5" s="0">
         <v>85.120000000000005</v>
@@ -1703,10 +2134,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>63</v>
+        <v>202</v>
       </c>
       <c r="C6" s="0">
-        <v>91.269999999999996</v>
+        <v>91.670000000000002</v>
       </c>
       <c r="D6" s="0">
         <v>100</v>
@@ -1742,7 +2173,7 @@
         <v>100</v>
       </c>
       <c r="O6" s="0">
-        <v>85.709999999999994</v>
+        <v>90.480000000000004</v>
       </c>
       <c r="P6" s="0">
         <v>21</v>
@@ -1753,7 +2184,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>64</v>
+        <v>203</v>
       </c>
       <c r="C7" s="0">
         <v>85.709999999999994</v>
@@ -1827,52 +2258,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>79</v>
+        <v>218</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>80</v>
+        <v>219</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>87</v>
+        <v>226</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>88</v>
+        <v>227</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>89</v>
+        <v>228</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>90</v>
+        <v>229</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>91</v>
+        <v>230</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>92</v>
+        <v>231</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>93</v>
+        <v>232</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>94</v>
+        <v>233</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>95</v>
+        <v>234</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>96</v>
+        <v>235</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>97</v>
+        <v>236</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>98</v>
+        <v>237</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>99</v>
+        <v>238</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>100</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2">
@@ -1880,7 +2311,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>81</v>
+        <v>220</v>
       </c>
       <c r="C2" s="0">
         <v>93.909999999999997</v>
@@ -1930,7 +2361,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>82</v>
+        <v>221</v>
       </c>
       <c r="C3" s="0">
         <v>91.030000000000001</v>
@@ -1980,7 +2411,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>83</v>
+        <v>222</v>
       </c>
       <c r="C4" s="0">
         <v>92.930000000000007</v>
@@ -2030,7 +2461,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>84</v>
+        <v>223</v>
       </c>
       <c r="C5" s="0">
         <v>80.060000000000002</v>
@@ -2080,10 +2511,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>85</v>
+        <v>224</v>
       </c>
       <c r="C6" s="0">
-        <v>90.480000000000004</v>
+        <v>90.870000000000005</v>
       </c>
       <c r="D6" s="0">
         <v>100</v>
@@ -2119,7 +2550,7 @@
         <v>100</v>
       </c>
       <c r="O6" s="0">
-        <v>90.480000000000004</v>
+        <v>95.239999999999995</v>
       </c>
       <c r="P6" s="0">
         <v>21</v>
@@ -2130,7 +2561,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>86</v>
+        <v>225</v>
       </c>
       <c r="C7" s="0">
         <v>80.560000000000002</v>
@@ -2204,52 +2635,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>101</v>
+        <v>240</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>102</v>
+        <v>241</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>109</v>
+        <v>248</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>110</v>
+        <v>249</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>111</v>
+        <v>250</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>112</v>
+        <v>251</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>113</v>
+        <v>252</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>114</v>
+        <v>253</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>115</v>
+        <v>254</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>116</v>
+        <v>255</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>117</v>
+        <v>256</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>118</v>
+        <v>257</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>119</v>
+        <v>258</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>120</v>
+        <v>259</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>121</v>
+        <v>260</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>122</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2">
@@ -2257,7 +2688,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>103</v>
+        <v>242</v>
       </c>
       <c r="C2" s="0">
         <v>96.150000000000006</v>
@@ -2307,7 +2738,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>104</v>
+        <v>243</v>
       </c>
       <c r="C3" s="0">
         <v>94.870000000000005</v>
@@ -2357,7 +2788,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>105</v>
+        <v>244</v>
       </c>
       <c r="C4" s="0">
         <v>94.439999999999998</v>
@@ -2407,7 +2838,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>106</v>
+        <v>245</v>
       </c>
       <c r="C5" s="0">
         <v>84.519999999999996</v>
@@ -2457,10 +2888,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>107</v>
+        <v>246</v>
       </c>
       <c r="C6" s="0">
-        <v>94.840000000000003</v>
+        <v>95.239999999999995</v>
       </c>
       <c r="D6" s="0">
         <v>100</v>
@@ -2496,7 +2927,7 @@
         <v>100</v>
       </c>
       <c r="O6" s="0">
-        <v>95.239999999999995</v>
+        <v>100</v>
       </c>
       <c r="P6" s="0">
         <v>21</v>
@@ -2507,7 +2938,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>108</v>
+        <v>247</v>
       </c>
       <c r="C7" s="0">
         <v>86.900000000000006</v>
@@ -2575,34 +3006,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>123</v>
+        <v>262</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>124</v>
+        <v>263</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>131</v>
+        <v>270</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>132</v>
+        <v>271</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>133</v>
+        <v>272</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>134</v>
+        <v>273</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>135</v>
+        <v>274</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>136</v>
+        <v>275</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>137</v>
+        <v>276</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>138</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2">
@@ -2610,7 +3041,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>125</v>
+        <v>264</v>
       </c>
       <c r="C2" s="0">
         <v>7.0499999999999998</v>
@@ -2642,7 +3073,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>126</v>
+        <v>265</v>
       </c>
       <c r="C3" s="0">
         <v>8.9700000000000006</v>
@@ -2674,7 +3105,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>127</v>
+        <v>266</v>
       </c>
       <c r="C4" s="0">
         <v>16.16</v>
@@ -2706,7 +3137,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>128</v>
+        <v>267</v>
       </c>
       <c r="C5" s="0">
         <v>10.710000000000001</v>
@@ -2738,7 +3169,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>129</v>
+        <v>268</v>
       </c>
       <c r="C6" s="0">
         <v>10.32</v>
@@ -2770,7 +3201,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>130</v>
+        <v>269</v>
       </c>
       <c r="C7" s="0">
         <v>4.7599999999999998</v>

</xml_diff>

<commit_message>
update AR (wrong order in L2); ET descriptive analysis; ET visualization started
</commit_message>
<xml_diff>
--- a/data/results/00_descriptiveResults_singleTC.xlsx
+++ b/data/results/00_descriptiveResults_singleTC.xlsx
@@ -20,7 +20,424 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="417">
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC02_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC03_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC04_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC05_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC06_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC07_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC08_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC09_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC10_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC11_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC12_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC06_AvailReasonCorrect_rel</t>
+  </si>
+  <si>
+    <t>TC10_AvailReasonCorrect_rel</t>
+  </si>
+  <si>
+    <t>TC12_AvailReasonCorrect_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC02_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC03_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC04_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC05_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC06_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC07_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC08_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC09_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC10_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC11_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC12_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC02_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC03_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC04_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC05_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC06_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC07_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC08_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC09_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC10_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC11_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC12_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC02_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC03_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC04_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC05_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC06_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC07_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC08_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC09_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC10_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC11_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC12_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC02_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC03_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC04_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC05_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC06_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC07_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC08_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC09_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC10_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC11_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC12_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC03_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC05_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC09_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC10_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC11_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC12_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
   <si>
     <t>Exp</t>
   </si>
@@ -874,7 +1291,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -896,11 +1313,18 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -916,6 +1340,13 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -948,52 +1379,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>139</v>
+        <v>278</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>140</v>
+        <v>279</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>147</v>
+        <v>286</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>148</v>
+        <v>287</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>149</v>
+        <v>288</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>150</v>
+        <v>289</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>151</v>
+        <v>290</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>152</v>
+        <v>291</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>153</v>
+        <v>292</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>154</v>
+        <v>293</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>155</v>
+        <v>294</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>156</v>
+        <v>295</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>157</v>
+        <v>296</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>158</v>
+        <v>297</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>159</v>
+        <v>298</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>160</v>
+        <v>299</v>
       </c>
     </row>
     <row r="2">
@@ -1001,7 +1432,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>141</v>
+        <v>280</v>
       </c>
       <c r="C2" s="0">
         <v>84.939999999999998</v>
@@ -1051,7 +1482,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>142</v>
+        <v>281</v>
       </c>
       <c r="C3" s="0">
         <v>84.939999999999998</v>
@@ -1101,7 +1532,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>143</v>
+        <v>282</v>
       </c>
       <c r="C4" s="0">
         <v>81.819999999999993</v>
@@ -1151,7 +1582,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>144</v>
+        <v>283</v>
       </c>
       <c r="C5" s="0">
         <v>74.700000000000003</v>
@@ -1201,7 +1632,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>145</v>
+        <v>284</v>
       </c>
       <c r="C6" s="0">
         <v>85.319999999999993</v>
@@ -1251,7 +1682,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>146</v>
+        <v>285</v>
       </c>
       <c r="C7" s="0">
         <v>71.430000000000007</v>
@@ -1316,25 +1747,25 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>161</v>
+        <v>300</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>162</v>
+        <v>301</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>169</v>
+        <v>308</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>170</v>
+        <v>309</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>171</v>
+        <v>310</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>172</v>
+        <v>311</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>173</v>
+        <v>312</v>
       </c>
     </row>
     <row r="2">
@@ -1342,7 +1773,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>163</v>
+        <v>302</v>
       </c>
       <c r="C2" s="0">
         <v>62.82</v>
@@ -1365,7 +1796,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>164</v>
+        <v>303</v>
       </c>
       <c r="C3" s="0">
         <v>75.640000000000001</v>
@@ -1388,7 +1819,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>165</v>
+        <v>304</v>
       </c>
       <c r="C4" s="0">
         <v>62.630000000000003</v>
@@ -1411,7 +1842,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>166</v>
+        <v>305</v>
       </c>
       <c r="C5" s="0">
         <v>55.950000000000003</v>
@@ -1434,7 +1865,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>167</v>
+        <v>306</v>
       </c>
       <c r="C6" s="0">
         <v>41.270000000000003</v>
@@ -1457,7 +1888,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>168</v>
+        <v>307</v>
       </c>
       <c r="C7" s="0">
         <v>23.809999999999999</v>
@@ -1504,52 +1935,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>174</v>
+        <v>313</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>175</v>
+        <v>314</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>182</v>
+        <v>321</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>183</v>
+        <v>322</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>184</v>
+        <v>323</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>185</v>
+        <v>324</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>186</v>
+        <v>325</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>187</v>
+        <v>326</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>188</v>
+        <v>327</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>189</v>
+        <v>328</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>190</v>
+        <v>329</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>191</v>
+        <v>330</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>192</v>
+        <v>331</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>193</v>
+        <v>332</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>194</v>
+        <v>333</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>195</v>
+        <v>334</v>
       </c>
     </row>
     <row r="2">
@@ -1557,7 +1988,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>176</v>
+        <v>315</v>
       </c>
       <c r="C2" s="0">
         <v>98.719999999999999</v>
@@ -1607,7 +2038,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>177</v>
+        <v>316</v>
       </c>
       <c r="C3" s="0">
         <v>97.120000000000005</v>
@@ -1657,7 +2088,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>178</v>
+        <v>317</v>
       </c>
       <c r="C4" s="0">
         <v>95.200000000000003</v>
@@ -1707,7 +2138,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>179</v>
+        <v>318</v>
       </c>
       <c r="C5" s="0">
         <v>87.5</v>
@@ -1757,7 +2188,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>180</v>
+        <v>319</v>
       </c>
       <c r="C6" s="0">
         <v>95.629999999999995</v>
@@ -1807,7 +2238,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>181</v>
+        <v>320</v>
       </c>
       <c r="C7" s="0">
         <v>84.920000000000002</v>
@@ -1881,52 +2312,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>196</v>
+        <v>335</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>197</v>
+        <v>336</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>204</v>
+        <v>343</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>205</v>
+        <v>344</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>206</v>
+        <v>345</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>207</v>
+        <v>346</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>208</v>
+        <v>347</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>209</v>
+        <v>348</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>210</v>
+        <v>349</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>211</v>
+        <v>350</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>212</v>
+        <v>351</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>213</v>
+        <v>352</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>214</v>
+        <v>353</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>215</v>
+        <v>354</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>216</v>
+        <v>355</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>217</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2">
@@ -1934,7 +2365,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>198</v>
+        <v>337</v>
       </c>
       <c r="C2" s="0">
         <v>98.719999999999999</v>
@@ -1984,7 +2415,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>199</v>
+        <v>338</v>
       </c>
       <c r="C3" s="0">
         <v>96.790000000000006</v>
@@ -2034,7 +2465,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>200</v>
+        <v>339</v>
       </c>
       <c r="C4" s="0">
         <v>90.400000000000006</v>
@@ -2084,7 +2515,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>201</v>
+        <v>340</v>
       </c>
       <c r="C5" s="0">
         <v>85.120000000000005</v>
@@ -2134,7 +2565,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>202</v>
+        <v>341</v>
       </c>
       <c r="C6" s="0">
         <v>91.670000000000002</v>
@@ -2184,7 +2615,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>203</v>
+        <v>342</v>
       </c>
       <c r="C7" s="0">
         <v>85.709999999999994</v>
@@ -2258,52 +2689,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>218</v>
+        <v>357</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>219</v>
+        <v>358</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>226</v>
+        <v>365</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>227</v>
+        <v>366</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>228</v>
+        <v>367</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>229</v>
+        <v>368</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>230</v>
+        <v>369</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>231</v>
+        <v>370</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>232</v>
+        <v>371</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>233</v>
+        <v>372</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>234</v>
+        <v>373</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>235</v>
+        <v>374</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>236</v>
+        <v>375</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>237</v>
+        <v>376</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>238</v>
+        <v>377</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>239</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2">
@@ -2311,7 +2742,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>220</v>
+        <v>359</v>
       </c>
       <c r="C2" s="0">
         <v>93.909999999999997</v>
@@ -2361,7 +2792,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>221</v>
+        <v>360</v>
       </c>
       <c r="C3" s="0">
         <v>91.030000000000001</v>
@@ -2411,7 +2842,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>222</v>
+        <v>361</v>
       </c>
       <c r="C4" s="0">
         <v>92.930000000000007</v>
@@ -2461,7 +2892,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>223</v>
+        <v>362</v>
       </c>
       <c r="C5" s="0">
         <v>80.060000000000002</v>
@@ -2511,7 +2942,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>224</v>
+        <v>363</v>
       </c>
       <c r="C6" s="0">
         <v>90.870000000000005</v>
@@ -2561,7 +2992,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>225</v>
+        <v>364</v>
       </c>
       <c r="C7" s="0">
         <v>80.560000000000002</v>
@@ -2635,52 +3066,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>240</v>
+        <v>379</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>241</v>
+        <v>380</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>248</v>
+        <v>387</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>249</v>
+        <v>388</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>250</v>
+        <v>389</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>251</v>
+        <v>390</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>252</v>
+        <v>391</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>253</v>
+        <v>392</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>254</v>
+        <v>393</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>255</v>
+        <v>394</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>256</v>
+        <v>395</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>257</v>
+        <v>396</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>258</v>
+        <v>397</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>259</v>
+        <v>398</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>260</v>
+        <v>399</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>261</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2">
@@ -2688,7 +3119,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>242</v>
+        <v>381</v>
       </c>
       <c r="C2" s="0">
         <v>96.150000000000006</v>
@@ -2738,7 +3169,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>243</v>
+        <v>382</v>
       </c>
       <c r="C3" s="0">
         <v>94.870000000000005</v>
@@ -2788,7 +3219,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>244</v>
+        <v>383</v>
       </c>
       <c r="C4" s="0">
         <v>94.439999999999998</v>
@@ -2838,7 +3269,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>245</v>
+        <v>384</v>
       </c>
       <c r="C5" s="0">
         <v>84.519999999999996</v>
@@ -2888,7 +3319,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>246</v>
+        <v>385</v>
       </c>
       <c r="C6" s="0">
         <v>95.239999999999995</v>
@@ -2938,7 +3369,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>247</v>
+        <v>386</v>
       </c>
       <c r="C7" s="0">
         <v>86.900000000000006</v>
@@ -3006,34 +3437,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>262</v>
+        <v>401</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>263</v>
+        <v>402</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>270</v>
+        <v>409</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>271</v>
+        <v>410</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>272</v>
+        <v>411</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>273</v>
+        <v>412</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>274</v>
+        <v>413</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>275</v>
+        <v>414</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>276</v>
+        <v>415</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>277</v>
+        <v>416</v>
       </c>
     </row>
     <row r="2">
@@ -3041,7 +3472,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>264</v>
+        <v>403</v>
       </c>
       <c r="C2" s="0">
         <v>7.0499999999999998</v>
@@ -3073,7 +3504,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>265</v>
+        <v>404</v>
       </c>
       <c r="C3" s="0">
         <v>8.9700000000000006</v>
@@ -3105,7 +3536,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>266</v>
+        <v>405</v>
       </c>
       <c r="C4" s="0">
         <v>16.16</v>
@@ -3137,7 +3568,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>267</v>
+        <v>406</v>
       </c>
       <c r="C5" s="0">
         <v>10.710000000000001</v>
@@ -3169,7 +3600,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>268</v>
+        <v>407</v>
       </c>
       <c r="C6" s="0">
         <v>10.32</v>
@@ -3201,7 +3632,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>269</v>
+        <v>408</v>
       </c>
       <c r="C7" s="0">
         <v>4.7599999999999998</v>

</xml_diff>

<commit_message>
DB descriptive analysis + DB visualization
</commit_message>
<xml_diff>
--- a/data/results/00_descriptiveResults_singleTC.xlsx
+++ b/data/results/00_descriptiveResults_singleTC.xlsx
@@ -20,7 +20,424 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="556">
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC02_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC03_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC04_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC05_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC06_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC07_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC08_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC09_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC10_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC11_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC12_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC06_AvailReasonCorrect_rel</t>
+  </si>
+  <si>
+    <t>TC10_AvailReasonCorrect_rel</t>
+  </si>
+  <si>
+    <t>TC12_AvailReasonCorrect_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC02_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC03_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC04_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC05_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC06_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC07_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC08_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC09_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC10_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC11_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC12_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC02_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC03_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC04_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC05_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC06_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC07_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC08_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC09_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC10_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC11_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC12_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC02_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC03_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC04_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC05_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC06_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC07_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC08_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC09_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC10_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC11_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC12_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC02_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC03_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC04_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC05_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC06_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC07_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC08_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC09_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC10_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC11_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC12_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC03_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC05_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC09_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC10_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC11_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC12_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
   <si>
     <t>Exp</t>
   </si>
@@ -1291,7 +1708,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -1320,11 +1737,18 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -1347,6 +1771,13 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1379,52 +1810,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>278</v>
+        <v>417</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>279</v>
+        <v>418</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>286</v>
+        <v>425</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>287</v>
+        <v>426</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>288</v>
+        <v>427</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>289</v>
+        <v>428</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>290</v>
+        <v>429</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>291</v>
+        <v>430</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>292</v>
+        <v>431</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>293</v>
+        <v>432</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>294</v>
+        <v>433</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>295</v>
+        <v>434</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>296</v>
+        <v>435</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>297</v>
+        <v>436</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>298</v>
+        <v>437</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>299</v>
+        <v>438</v>
       </c>
     </row>
     <row r="2">
@@ -1432,7 +1863,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>280</v>
+        <v>419</v>
       </c>
       <c r="C2" s="0">
         <v>84.939999999999998</v>
@@ -1482,7 +1913,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>281</v>
+        <v>420</v>
       </c>
       <c r="C3" s="0">
         <v>84.939999999999998</v>
@@ -1532,7 +1963,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>282</v>
+        <v>421</v>
       </c>
       <c r="C4" s="0">
         <v>81.819999999999993</v>
@@ -1582,7 +2013,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>283</v>
+        <v>422</v>
       </c>
       <c r="C5" s="0">
         <v>74.700000000000003</v>
@@ -1632,7 +2063,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>284</v>
+        <v>423</v>
       </c>
       <c r="C6" s="0">
         <v>85.319999999999993</v>
@@ -1682,7 +2113,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>285</v>
+        <v>424</v>
       </c>
       <c r="C7" s="0">
         <v>71.430000000000007</v>
@@ -1747,25 +2178,25 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>300</v>
+        <v>439</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>301</v>
+        <v>440</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>308</v>
+        <v>447</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>309</v>
+        <v>448</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>310</v>
+        <v>449</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>311</v>
+        <v>450</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>312</v>
+        <v>451</v>
       </c>
     </row>
     <row r="2">
@@ -1773,7 +2204,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>302</v>
+        <v>441</v>
       </c>
       <c r="C2" s="0">
         <v>62.82</v>
@@ -1796,7 +2227,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>303</v>
+        <v>442</v>
       </c>
       <c r="C3" s="0">
         <v>75.640000000000001</v>
@@ -1819,7 +2250,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>304</v>
+        <v>443</v>
       </c>
       <c r="C4" s="0">
         <v>62.630000000000003</v>
@@ -1842,7 +2273,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>305</v>
+        <v>444</v>
       </c>
       <c r="C5" s="0">
         <v>55.950000000000003</v>
@@ -1865,7 +2296,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>306</v>
+        <v>445</v>
       </c>
       <c r="C6" s="0">
         <v>41.270000000000003</v>
@@ -1888,7 +2319,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>307</v>
+        <v>446</v>
       </c>
       <c r="C7" s="0">
         <v>23.809999999999999</v>
@@ -1935,52 +2366,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>313</v>
+        <v>452</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>314</v>
+        <v>453</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>321</v>
+        <v>460</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>322</v>
+        <v>461</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>323</v>
+        <v>462</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>324</v>
+        <v>463</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>325</v>
+        <v>464</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>326</v>
+        <v>465</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>327</v>
+        <v>466</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>328</v>
+        <v>467</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>329</v>
+        <v>468</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>330</v>
+        <v>469</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>331</v>
+        <v>470</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>332</v>
+        <v>471</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>333</v>
+        <v>472</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>334</v>
+        <v>473</v>
       </c>
     </row>
     <row r="2">
@@ -1988,7 +2419,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>315</v>
+        <v>454</v>
       </c>
       <c r="C2" s="0">
         <v>98.719999999999999</v>
@@ -2038,7 +2469,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>316</v>
+        <v>455</v>
       </c>
       <c r="C3" s="0">
         <v>97.120000000000005</v>
@@ -2088,7 +2519,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>317</v>
+        <v>456</v>
       </c>
       <c r="C4" s="0">
         <v>95.200000000000003</v>
@@ -2138,7 +2569,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>318</v>
+        <v>457</v>
       </c>
       <c r="C5" s="0">
         <v>87.5</v>
@@ -2188,7 +2619,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>319</v>
+        <v>458</v>
       </c>
       <c r="C6" s="0">
         <v>95.629999999999995</v>
@@ -2238,7 +2669,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>320</v>
+        <v>459</v>
       </c>
       <c r="C7" s="0">
         <v>84.920000000000002</v>
@@ -2312,52 +2743,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>335</v>
+        <v>474</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>336</v>
+        <v>475</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>343</v>
+        <v>482</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>344</v>
+        <v>483</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>345</v>
+        <v>484</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>346</v>
+        <v>485</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>347</v>
+        <v>486</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>348</v>
+        <v>487</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>349</v>
+        <v>488</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>350</v>
+        <v>489</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>351</v>
+        <v>490</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>352</v>
+        <v>491</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>353</v>
+        <v>492</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>354</v>
+        <v>493</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>355</v>
+        <v>494</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>356</v>
+        <v>495</v>
       </c>
     </row>
     <row r="2">
@@ -2365,7 +2796,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>337</v>
+        <v>476</v>
       </c>
       <c r="C2" s="0">
         <v>98.719999999999999</v>
@@ -2415,7 +2846,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>338</v>
+        <v>477</v>
       </c>
       <c r="C3" s="0">
         <v>96.790000000000006</v>
@@ -2465,7 +2896,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>339</v>
+        <v>478</v>
       </c>
       <c r="C4" s="0">
         <v>90.400000000000006</v>
@@ -2515,7 +2946,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>340</v>
+        <v>479</v>
       </c>
       <c r="C5" s="0">
         <v>85.120000000000005</v>
@@ -2565,7 +2996,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>341</v>
+        <v>480</v>
       </c>
       <c r="C6" s="0">
         <v>91.670000000000002</v>
@@ -2615,7 +3046,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>342</v>
+        <v>481</v>
       </c>
       <c r="C7" s="0">
         <v>85.709999999999994</v>
@@ -2689,52 +3120,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>357</v>
+        <v>496</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>358</v>
+        <v>497</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>365</v>
+        <v>504</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>366</v>
+        <v>505</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>367</v>
+        <v>506</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>368</v>
+        <v>507</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>369</v>
+        <v>508</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>370</v>
+        <v>509</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>371</v>
+        <v>510</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>372</v>
+        <v>511</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>373</v>
+        <v>512</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>374</v>
+        <v>513</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>375</v>
+        <v>514</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>376</v>
+        <v>515</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>377</v>
+        <v>516</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>378</v>
+        <v>517</v>
       </c>
     </row>
     <row r="2">
@@ -2742,7 +3173,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>359</v>
+        <v>498</v>
       </c>
       <c r="C2" s="0">
         <v>93.909999999999997</v>
@@ -2792,7 +3223,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>360</v>
+        <v>499</v>
       </c>
       <c r="C3" s="0">
         <v>91.030000000000001</v>
@@ -2842,7 +3273,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>361</v>
+        <v>500</v>
       </c>
       <c r="C4" s="0">
         <v>92.930000000000007</v>
@@ -2892,7 +3323,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>362</v>
+        <v>501</v>
       </c>
       <c r="C5" s="0">
         <v>80.060000000000002</v>
@@ -2942,7 +3373,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>363</v>
+        <v>502</v>
       </c>
       <c r="C6" s="0">
         <v>90.870000000000005</v>
@@ -2992,7 +3423,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>364</v>
+        <v>503</v>
       </c>
       <c r="C7" s="0">
         <v>80.560000000000002</v>
@@ -3066,52 +3497,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>379</v>
+        <v>518</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>380</v>
+        <v>519</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>387</v>
+        <v>526</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>388</v>
+        <v>527</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>389</v>
+        <v>528</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>390</v>
+        <v>529</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>391</v>
+        <v>530</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>392</v>
+        <v>531</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>393</v>
+        <v>532</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>394</v>
+        <v>533</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>395</v>
+        <v>534</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>396</v>
+        <v>535</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>397</v>
+        <v>536</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>398</v>
+        <v>537</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>399</v>
+        <v>538</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>400</v>
+        <v>539</v>
       </c>
     </row>
     <row r="2">
@@ -3119,7 +3550,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>381</v>
+        <v>520</v>
       </c>
       <c r="C2" s="0">
         <v>96.150000000000006</v>
@@ -3169,7 +3600,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>382</v>
+        <v>521</v>
       </c>
       <c r="C3" s="0">
         <v>94.870000000000005</v>
@@ -3219,7 +3650,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>383</v>
+        <v>522</v>
       </c>
       <c r="C4" s="0">
         <v>94.439999999999998</v>
@@ -3269,7 +3700,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>384</v>
+        <v>523</v>
       </c>
       <c r="C5" s="0">
         <v>84.519999999999996</v>
@@ -3319,7 +3750,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>385</v>
+        <v>524</v>
       </c>
       <c r="C6" s="0">
         <v>95.239999999999995</v>
@@ -3369,7 +3800,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>386</v>
+        <v>525</v>
       </c>
       <c r="C7" s="0">
         <v>86.900000000000006</v>
@@ -3437,34 +3868,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>401</v>
+        <v>540</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>402</v>
+        <v>541</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>409</v>
+        <v>548</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>410</v>
+        <v>549</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>411</v>
+        <v>550</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>412</v>
+        <v>551</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>413</v>
+        <v>552</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>414</v>
+        <v>553</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>415</v>
+        <v>554</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>416</v>
+        <v>555</v>
       </c>
     </row>
     <row r="2">
@@ -3472,7 +3903,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>403</v>
+        <v>542</v>
       </c>
       <c r="C2" s="0">
         <v>7.0499999999999998</v>
@@ -3504,7 +3935,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>404</v>
+        <v>543</v>
       </c>
       <c r="C3" s="0">
         <v>8.9700000000000006</v>
@@ -3536,7 +3967,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>405</v>
+        <v>544</v>
       </c>
       <c r="C4" s="0">
         <v>16.16</v>
@@ -3568,7 +3999,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>406</v>
+        <v>545</v>
       </c>
       <c r="C5" s="0">
         <v>10.710000000000001</v>
@@ -3600,7 +4031,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>407</v>
+        <v>546</v>
       </c>
       <c r="C6" s="0">
         <v>10.32</v>
@@ -3632,7 +4063,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>408</v>
+        <v>547</v>
       </c>
       <c r="C7" s="0">
         <v>4.7599999999999998</v>

</xml_diff>

<commit_message>
n_metrics, usability_ratings, conclusions, update ET
</commit_message>
<xml_diff>
--- a/data/results/00_descriptiveResults_singleTC.xlsx
+++ b/data/results/00_descriptiveResults_singleTC.xlsx
@@ -20,7 +20,1675 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="1112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1668" uniqueCount="1668">
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC02_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC03_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC04_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC05_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC06_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC07_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC08_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC09_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC10_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC11_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC12_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC06_AvailReasonCorrect_rel</t>
+  </si>
+  <si>
+    <t>TC10_AvailReasonCorrect_rel</t>
+  </si>
+  <si>
+    <t>TC12_AvailReasonCorrect_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC02_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC03_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC04_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC05_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC06_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC07_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC08_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC09_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC10_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC11_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC12_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC02_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC03_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC04_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC05_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC06_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC07_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC08_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC09_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC10_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC11_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC12_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC02_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC03_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC04_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC05_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC06_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC07_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC08_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC09_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC10_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC11_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC12_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC02_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC03_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC04_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC05_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC06_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC07_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC08_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC09_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC10_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC11_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC12_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC03_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC05_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC09_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC10_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC11_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC12_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC02_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC03_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC04_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC05_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC06_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC07_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC08_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC09_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC10_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC11_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC12_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC06_AvailReasonCorrect_rel</t>
+  </si>
+  <si>
+    <t>TC10_AvailReasonCorrect_rel</t>
+  </si>
+  <si>
+    <t>TC12_AvailReasonCorrect_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC02_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC03_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC04_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC05_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC06_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC07_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC08_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC09_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC10_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC11_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC12_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC02_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC03_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC04_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC05_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC06_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC07_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC08_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC09_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC10_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC11_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC12_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC02_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC03_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC04_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC05_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC06_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC07_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC08_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC09_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC10_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC11_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC12_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC02_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC03_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC04_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC05_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC06_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC07_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC08_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC09_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC10_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC11_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC12_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC03_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC05_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC09_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC10_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC11_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC12_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC02_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC03_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC04_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC05_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC06_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC07_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC08_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC09_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC10_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC11_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC12_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC06_AvailReasonCorrect_rel</t>
+  </si>
+  <si>
+    <t>TC10_AvailReasonCorrect_rel</t>
+  </si>
+  <si>
+    <t>TC12_AvailReasonCorrect_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC02_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC03_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC04_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC05_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC06_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC07_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC08_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC09_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC10_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC11_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC12_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC02_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC03_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC04_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC05_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC06_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC07_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC08_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC09_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC10_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC11_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC12_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC02_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC03_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC04_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC05_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC06_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC07_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC08_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC09_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC10_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC11_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC12_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC02_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC03_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC04_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC05_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC06_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC07_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC08_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC09_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC10_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC11_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC12_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC03_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC05_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC09_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC10_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC11_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC12_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC02_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC03_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC04_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC05_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC06_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC07_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC08_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC09_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC10_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC11_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC12_AvailImplem_Rep_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC06_AvailReasonCorrect_rel</t>
+  </si>
+  <si>
+    <t>TC10_AvailReasonCorrect_rel</t>
+  </si>
+  <si>
+    <t>TC12_AvailReasonCorrect_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC02_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC03_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC04_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC05_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC06_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC07_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC08_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC09_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC10_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC11_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC12_EmailsAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC02_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC03_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC04_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC05_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC06_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC07_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC08_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC09_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC10_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC11_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>TC12_HandsOffAllow_Observed_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC02_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC03_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC04_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC05_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC06_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC07_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC08_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC09_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC10_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC11_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>TC12_LevelObserved_Instr_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC01_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC02_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC03_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC04_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC05_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC06_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC07_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC08_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC09_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC10_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC11_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>TC12_LevelObserved_Rep_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>HMI</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>HC</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>TC03_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC05_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC09_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC10_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC11_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>TC12_TransProblems_rel</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
   <si>
     <t>Exp</t>
   </si>
@@ -3376,7 +5044,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="57">
+  <borders count="85">
     <border>
       <left/>
       <right/>
@@ -3440,11 +5108,39 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -3502,6 +5198,34 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="55" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="57" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="58" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="59" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="60" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="61" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="62" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="63" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="64" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="65" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="66" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="67" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="68" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="69" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="70" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="71" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="72" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="73" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="74" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="75" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="76" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="77" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="78" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="79" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="80" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="81" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="82" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="83" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="84" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3534,52 +5258,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>973</v>
+        <v>1529</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>974</v>
+        <v>1530</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>981</v>
+        <v>1537</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>982</v>
+        <v>1538</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>983</v>
+        <v>1539</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>984</v>
+        <v>1540</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>985</v>
+        <v>1541</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>986</v>
+        <v>1542</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>987</v>
+        <v>1543</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>988</v>
+        <v>1544</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>989</v>
+        <v>1545</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>990</v>
+        <v>1546</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>991</v>
+        <v>1547</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>992</v>
+        <v>1548</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>993</v>
+        <v>1549</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>994</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="2">
@@ -3587,7 +5311,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>975</v>
+        <v>1531</v>
       </c>
       <c r="C2" s="0">
         <v>84.939999999999998</v>
@@ -3637,7 +5361,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>976</v>
+        <v>1532</v>
       </c>
       <c r="C3" s="0">
         <v>84.939999999999998</v>
@@ -3687,7 +5411,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>977</v>
+        <v>1533</v>
       </c>
       <c r="C4" s="0">
         <v>81.819999999999993</v>
@@ -3737,7 +5461,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>978</v>
+        <v>1534</v>
       </c>
       <c r="C5" s="0">
         <v>74.700000000000003</v>
@@ -3787,7 +5511,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>979</v>
+        <v>1535</v>
       </c>
       <c r="C6" s="0">
         <v>85.319999999999993</v>
@@ -3837,7 +5561,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>980</v>
+        <v>1536</v>
       </c>
       <c r="C7" s="0">
         <v>71.430000000000007</v>
@@ -3902,25 +5626,25 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>995</v>
+        <v>1551</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>996</v>
+        <v>1552</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1003</v>
+        <v>1559</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>1004</v>
+        <v>1560</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>1005</v>
+        <v>1561</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>1006</v>
+        <v>1562</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>1007</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="2">
@@ -3928,7 +5652,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>997</v>
+        <v>1553</v>
       </c>
       <c r="C2" s="0">
         <v>62.82</v>
@@ -3951,7 +5675,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>998</v>
+        <v>1554</v>
       </c>
       <c r="C3" s="0">
         <v>75.640000000000001</v>
@@ -3974,7 +5698,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>999</v>
+        <v>1555</v>
       </c>
       <c r="C4" s="0">
         <v>62.630000000000003</v>
@@ -3997,7 +5721,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>1000</v>
+        <v>1556</v>
       </c>
       <c r="C5" s="0">
         <v>55.950000000000003</v>
@@ -4020,7 +5744,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>1001</v>
+        <v>1557</v>
       </c>
       <c r="C6" s="0">
         <v>41.270000000000003</v>
@@ -4043,7 +5767,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>1002</v>
+        <v>1558</v>
       </c>
       <c r="C7" s="0">
         <v>23.809999999999999</v>
@@ -4090,52 +5814,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>1008</v>
+        <v>1564</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1009</v>
+        <v>1565</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1016</v>
+        <v>1572</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>1017</v>
+        <v>1573</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>1018</v>
+        <v>1574</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>1019</v>
+        <v>1575</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>1020</v>
+        <v>1576</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>1021</v>
+        <v>1577</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>1022</v>
+        <v>1578</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>1023</v>
+        <v>1579</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>1024</v>
+        <v>1580</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>1025</v>
+        <v>1581</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>1026</v>
+        <v>1582</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>1027</v>
+        <v>1583</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>1028</v>
+        <v>1584</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>1029</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="2">
@@ -4143,7 +5867,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>1010</v>
+        <v>1566</v>
       </c>
       <c r="C2" s="0">
         <v>98.719999999999999</v>
@@ -4193,7 +5917,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>1011</v>
+        <v>1567</v>
       </c>
       <c r="C3" s="0">
         <v>97.120000000000005</v>
@@ -4243,7 +5967,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>1012</v>
+        <v>1568</v>
       </c>
       <c r="C4" s="0">
         <v>95.200000000000003</v>
@@ -4293,7 +6017,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>1013</v>
+        <v>1569</v>
       </c>
       <c r="C5" s="0">
         <v>87.5</v>
@@ -4343,7 +6067,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>1014</v>
+        <v>1570</v>
       </c>
       <c r="C6" s="0">
         <v>95.629999999999995</v>
@@ -4393,7 +6117,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>1015</v>
+        <v>1571</v>
       </c>
       <c r="C7" s="0">
         <v>84.920000000000002</v>
@@ -4467,52 +6191,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>1030</v>
+        <v>1586</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1031</v>
+        <v>1587</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1038</v>
+        <v>1594</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>1039</v>
+        <v>1595</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>1040</v>
+        <v>1596</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>1041</v>
+        <v>1597</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>1042</v>
+        <v>1598</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>1043</v>
+        <v>1599</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>1044</v>
+        <v>1600</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>1045</v>
+        <v>1601</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>1046</v>
+        <v>1602</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>1047</v>
+        <v>1603</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>1048</v>
+        <v>1604</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>1049</v>
+        <v>1605</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>1050</v>
+        <v>1606</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>1051</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="2">
@@ -4520,7 +6244,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>1032</v>
+        <v>1588</v>
       </c>
       <c r="C2" s="0">
         <v>98.719999999999999</v>
@@ -4570,7 +6294,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>1033</v>
+        <v>1589</v>
       </c>
       <c r="C3" s="0">
         <v>96.790000000000006</v>
@@ -4620,7 +6344,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>1034</v>
+        <v>1590</v>
       </c>
       <c r="C4" s="0">
         <v>90.400000000000006</v>
@@ -4670,7 +6394,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>1035</v>
+        <v>1591</v>
       </c>
       <c r="C5" s="0">
         <v>85.120000000000005</v>
@@ -4720,7 +6444,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>1036</v>
+        <v>1592</v>
       </c>
       <c r="C6" s="0">
         <v>91.670000000000002</v>
@@ -4770,7 +6494,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>1037</v>
+        <v>1593</v>
       </c>
       <c r="C7" s="0">
         <v>85.709999999999994</v>
@@ -4844,52 +6568,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>1052</v>
+        <v>1608</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1053</v>
+        <v>1609</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1060</v>
+        <v>1616</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>1061</v>
+        <v>1617</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>1062</v>
+        <v>1618</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>1063</v>
+        <v>1619</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>1064</v>
+        <v>1620</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>1065</v>
+        <v>1621</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>1066</v>
+        <v>1622</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>1067</v>
+        <v>1623</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>1068</v>
+        <v>1624</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>1069</v>
+        <v>1625</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>1070</v>
+        <v>1626</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>1071</v>
+        <v>1627</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>1072</v>
+        <v>1628</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>1073</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="2">
@@ -4897,7 +6621,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>1054</v>
+        <v>1610</v>
       </c>
       <c r="C2" s="0">
         <v>93.909999999999997</v>
@@ -4947,7 +6671,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>1055</v>
+        <v>1611</v>
       </c>
       <c r="C3" s="0">
         <v>91.030000000000001</v>
@@ -4997,7 +6721,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>1056</v>
+        <v>1612</v>
       </c>
       <c r="C4" s="0">
         <v>92.930000000000007</v>
@@ -5047,7 +6771,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>1057</v>
+        <v>1613</v>
       </c>
       <c r="C5" s="0">
         <v>80.060000000000002</v>
@@ -5097,7 +6821,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>1058</v>
+        <v>1614</v>
       </c>
       <c r="C6" s="0">
         <v>90.870000000000005</v>
@@ -5147,7 +6871,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>1059</v>
+        <v>1615</v>
       </c>
       <c r="C7" s="0">
         <v>80.560000000000002</v>
@@ -5221,52 +6945,52 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>1074</v>
+        <v>1630</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1075</v>
+        <v>1631</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1082</v>
+        <v>1638</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>1083</v>
+        <v>1639</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>1084</v>
+        <v>1640</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>1085</v>
+        <v>1641</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>1086</v>
+        <v>1642</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>1087</v>
+        <v>1643</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>1088</v>
+        <v>1644</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>1089</v>
+        <v>1645</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>1090</v>
+        <v>1646</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>1091</v>
+        <v>1647</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>1092</v>
+        <v>1648</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>1093</v>
+        <v>1649</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>1094</v>
+        <v>1650</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>1095</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="2">
@@ -5274,7 +6998,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>1076</v>
+        <v>1632</v>
       </c>
       <c r="C2" s="0">
         <v>96.150000000000006</v>
@@ -5324,7 +7048,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>1077</v>
+        <v>1633</v>
       </c>
       <c r="C3" s="0">
         <v>94.870000000000005</v>
@@ -5374,7 +7098,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>1078</v>
+        <v>1634</v>
       </c>
       <c r="C4" s="0">
         <v>94.439999999999998</v>
@@ -5424,7 +7148,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>1079</v>
+        <v>1635</v>
       </c>
       <c r="C5" s="0">
         <v>84.519999999999996</v>
@@ -5474,7 +7198,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>1080</v>
+        <v>1636</v>
       </c>
       <c r="C6" s="0">
         <v>95.239999999999995</v>
@@ -5524,7 +7248,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>1081</v>
+        <v>1637</v>
       </c>
       <c r="C7" s="0">
         <v>86.900000000000006</v>
@@ -5592,34 +7316,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>1096</v>
+        <v>1652</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1097</v>
+        <v>1653</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1104</v>
+        <v>1660</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>1105</v>
+        <v>1661</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>1106</v>
+        <v>1662</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>1107</v>
+        <v>1663</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>1108</v>
+        <v>1664</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>1109</v>
+        <v>1665</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>1110</v>
+        <v>1666</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>1111</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="2">
@@ -5627,7 +7351,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>1098</v>
+        <v>1654</v>
       </c>
       <c r="C2" s="0">
         <v>7.0499999999999998</v>
@@ -5659,7 +7383,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>1099</v>
+        <v>1655</v>
       </c>
       <c r="C3" s="0">
         <v>8.9700000000000006</v>
@@ -5691,7 +7415,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>1100</v>
+        <v>1656</v>
       </c>
       <c r="C4" s="0">
         <v>16.16</v>
@@ -5723,7 +7447,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>1101</v>
+        <v>1657</v>
       </c>
       <c r="C5" s="0">
         <v>10.710000000000001</v>
@@ -5755,7 +7479,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>1102</v>
+        <v>1658</v>
       </c>
       <c r="C6" s="0">
         <v>10.32</v>
@@ -5787,7 +7511,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>1103</v>
+        <v>1659</v>
       </c>
       <c r="C7" s="0">
         <v>4.7599999999999998</v>

</xml_diff>